<commit_message>
Caixa para Deck Commander - Satoru Umezawa
</commit_message>
<xml_diff>
--- a/Pedidos/Planilha-de-custos-impressao-3D.xlsx
+++ b/Pedidos/Planilha-de-custos-impressao-3D.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josue\Desktop\Pedidos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josue\Desktop\Soir Alliv\Pedidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C25BC41-C37E-4721-BE0A-2961F5F1C2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55A2320-A880-4007-AE5D-0CD7496FB101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5666" yWindow="2760" windowWidth="10020" windowHeight="13054" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6009" yWindow="3103" windowWidth="10020" windowHeight="13054" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CUSTO" sheetId="1" r:id="rId1"/>
@@ -647,7 +647,7 @@
   <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>9</v>
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="4" t="s">
@@ -715,7 +715,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="2" t="s">
@@ -773,7 +773,7 @@
       </c>
       <c r="D9" s="3">
         <f>(D3/1000)*D4</f>
-        <v>19.8</v>
+        <v>14</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="2" t="s">
@@ -790,7 +790,7 @@
       </c>
       <c r="D10" s="3">
         <f>((D6*D7)/1000)*D5</f>
-        <v>4.2876000000000003</v>
+        <v>2.8584000000000005</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -800,7 +800,7 @@
       </c>
       <c r="D11" s="8">
         <f>D9+D10</f>
-        <v>24.087600000000002</v>
+        <v>16.8584</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>10</v>
@@ -849,7 +849,7 @@
       </c>
       <c r="D14" s="14">
         <f>(D11*D13)+D11</f>
-        <v>60.219000000000001</v>
+        <v>42.146000000000001</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="4" t="s">
@@ -865,7 +865,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="11">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="7" t="s">
@@ -883,7 +883,7 @@
       </c>
       <c r="D16" s="16">
         <f>D15-D11</f>
-        <v>45.912399999999998</v>
+        <v>28.1416</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.4">

</xml_diff>